<commit_message>
addded iris dataset notebook
</commit_message>
<xml_diff>
--- a/Todo and Excel Trackers/Tracker.xlsx
+++ b/Todo and Excel Trackers/Tracker.xlsx
@@ -25,9 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>https://www.datacamp.com/community/tutorials/machine-learning-python</t>
+  </si>
+  <si>
+    <t>All Harward lectures CS109</t>
+  </si>
+  <si>
+    <t>For practical strated with Iris dataset</t>
   </si>
 </sst>
 </file>
@@ -353,17 +359,23 @@
   <cols>
     <col min="1" max="1" width="43.140625" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -373,7 +385,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ufo dataset from Acloud guru
</commit_message>
<xml_diff>
--- a/Todo and Excel Trackers/Tracker.xlsx
+++ b/Todo and Excel Trackers/Tracker.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Python\All-Machine-Learning\Todo and Excel Trackers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hrushi\Python\ML\All-Machine-Learning\Todo and Excel Trackers\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617A5A8A-1846-4658-BF8B-7157D2AFD7CC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Useful Websites" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>https://www.datacamp.com/community/tutorials/machine-learning-python</t>
   </si>
@@ -34,14 +35,43 @@
   </si>
   <si>
     <t>For practical strated with Iris dataset</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Complete credit-fraud-dealing-with-imbalanced-datasets - https://www.kaggle.com/janiobachmann/credit-fraud-dealing-with-imbalanced-datasets</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Do a spark/Datbricks Project</t>
+  </si>
+  <si>
+    <t>Understand PCA blood and bone means corrctly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -69,8 +99,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -350,50 +385,98 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="43.140625" customWidth="1"/>
+    <col min="1" max="1" width="43.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="70.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3">
+        <v>43790</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3">
+        <v>43790</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3">
+        <v>43790</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>